<commit_message>
feat: update data ufter perbaharui
</commit_message>
<xml_diff>
--- a/upload/file.xlsx
+++ b/upload/file.xlsx
@@ -163,7 +163,7 @@
     <t xml:space="preserve">26-11-2021 01:28:46</t>
   </si>
   <si>
-    <t xml:space="preserve">Saiting</t>
+    <t xml:space="preserve">Saitin</t>
   </si>
   <si>
     <t xml:space="preserve">Bapak Septian</t>
@@ -193,7 +193,7 @@
     <t xml:space="preserve">25-11-2021 22:22:31</t>
   </si>
   <si>
-    <t xml:space="preserve">selesai</t>
+    <t xml:space="preserve">selass</t>
   </si>
   <si>
     <t xml:space="preserve">Pak Badri</t>
@@ -306,7 +306,7 @@
   </sheetPr>
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>

</xml_diff>